<commit_message>
Upd reports: Add 1 annotator, F1-Pos Diff correlation to annotation_error
</commit_message>
<xml_diff>
--- a/reports/annotation_error.xlsx
+++ b/reports/annotation_error.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Arquivos Incomuns\Projeto Final\semiauto-video-annotation\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D712A5D3-7EBA-42C0-A63A-6609E505CD68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A21A03-5712-449E-A612-EE6E152C46DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{72EED3A8-5827-40EA-B63F-F09D88BB37DC}"/>
   </bookViews>
@@ -32,14 +32,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={7B74CFFE-0348-48B1-9693-0C0336A61E4A}</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{7B74CFFE-0348-48B1-9693-0C0336A61E4A}">
+      <text>
+        <t>[Comentário encadeado]
+Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
+Comentário:
+    anotado apenas pelo Felipe</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Semiauto/Ref</t>
-  </si>
-  <si>
-    <t>Correlation</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Event</t>
   </si>
@@ -62,29 +74,61 @@
     <t>Repair</t>
   </si>
   <si>
-    <t>Labeling error %</t>
-  </si>
-  <si>
     <t>F1 Score</t>
   </si>
   <si>
     <t>Level</t>
+  </si>
+  <si>
+    <t>Correlation F1-Labeling Error</t>
+  </si>
+  <si>
+    <t>Correlation F1-Positive Diff</t>
+  </si>
+  <si>
+    <t>Labeling error % (Felipe)</t>
+  </si>
+  <si>
+    <t>Labeling error % (Karen)</t>
+  </si>
+  <si>
+    <t>Labeling error % (Avg)</t>
+  </si>
+  <si>
+    <t>Positive Auto-Manual % diff</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Semiauto dataset</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0%"/>
-  </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -107,16 +151,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -132,6 +178,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Olavo Sampaio" id="{D90A1C48-A4EB-4D14-A32A-2C5063C9920C}" userId="5dc859e3f5210d34" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -429,130 +481,272 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B2" dT="2020-03-04T02:06:48.55" personId="{D90A1C48-A4EB-4D14-A32A-2C5063C9920C}" id="{7B74CFFE-0348-48B1-9693-0C0336A61E4A}">
+    <text>anotado apenas pelo Felipe</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{340C8B92-D602-4102-907F-D1A3B217CB79}">
-  <dimension ref="A1:G8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{340C8B92-D602-4102-907F-D1A3B217CB79}">
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1">
+        <f>CORREL(E2:E8,F2:F8)</f>
+        <v>-0.78913108839245982</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>7.5700000000000003E-2</v>
+      </c>
+      <c r="D2" s="5">
+        <v>7.5700000000000003E-2</v>
+      </c>
+      <c r="E2" s="5">
+        <f>AVERAGE(C2:D2)</f>
+        <v>7.5700000000000003E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.93598862019914653</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1">
+        <f>CORREL(F2:F8,G2:G8)</f>
+        <v>-0.82343097722801939</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1">
-        <f>CORREL(C2:C10,D2:D10)</f>
-        <v>-0.79828469902360299</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2">
-        <v>7.5700000000000003E-2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.93598862019914653</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="C3" s="5">
+        <v>0.10059999999999999</v>
+      </c>
+      <c r="D3" s="5">
         <v>0.1205</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E8" si="0">AVERAGE(C3:D3)</f>
+        <v>0.11055</v>
+      </c>
+      <c r="F3" s="1">
         <v>0.87889273356401376</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G3" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2.4400000000000002E-2</v>
+      </c>
+      <c r="D4" s="5">
         <v>3.7499999999999999E-2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="5">
+        <f t="shared" si="0"/>
+        <v>3.0949999999999998E-2</v>
+      </c>
+      <c r="F4" s="1">
         <v>0.69699999999999995</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G4" s="4">
+        <v>3.0765086669152203E-2</v>
+      </c>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.1452</v>
+      </c>
+      <c r="D5" s="5">
         <v>0.2102</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="5">
+        <f t="shared" si="0"/>
+        <v>0.1777</v>
+      </c>
+      <c r="F5" s="1">
         <v>0.41299999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G5" s="4">
+        <v>0.32173350150617291</v>
+      </c>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5">
+        <v>5.3400000000000003E-2</v>
+      </c>
+      <c r="D6" s="5">
         <v>0.1386</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="5">
+        <f t="shared" si="0"/>
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="F6" s="1">
         <v>0.81100000000000005</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G6" s="4">
+        <v>0.26669531662415558</v>
+      </c>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.11849999999999999</v>
+      </c>
+      <c r="D7" s="5">
         <v>6.88E-2</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="5">
+        <f t="shared" si="0"/>
+        <v>9.3649999999999997E-2</v>
+      </c>
+      <c r="F7" s="1">
         <v>0.72899999999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G7" s="4">
+        <v>0.24805868053601665</v>
+      </c>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2">
+        <v>6</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.95109999999999995</v>
+      </c>
+      <c r="D8" s="5">
         <v>0.94530000000000003</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.94819999999999993</v>
+      </c>
+      <c r="F8" s="1">
         <v>0.247</v>
       </c>
+      <c r="G8" s="4">
+        <v>0.74578678005320553</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H12" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H15" s="4"/>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H18" s="4"/>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H21" s="4"/>
+    </row>
+    <row r="23" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H24" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -560,5 +754,6 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>